<commit_message>
New groups and video link
</commit_message>
<xml_diff>
--- a/project/P0-pick-papers/PaperChoices.xlsx
+++ b/project/P0-pick-papers/PaperChoices.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PaperList" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>Study</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t>Chris Klocke</t>
+  </si>
+  <si>
+    <t>Austin Nguyen</t>
+  </si>
+  <si>
+    <t>Colleen Xu</t>
+  </si>
+  <si>
+    <t>Xiao Wang</t>
   </si>
 </sst>
 </file>
@@ -1256,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,6 +1356,30 @@
         <v>60</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1354,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,6 +1510,39 @@
         <v>7</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated PaperChoices and added notes to due.
</commit_message>
<xml_diff>
--- a/project/P0-pick-papers/PaperChoices.xlsx
+++ b/project/P0-pick-papers/PaperChoices.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" tabRatio="706"/>
   </bookViews>
   <sheets>
     <sheet name="PaperList" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="100">
   <si>
     <t>Study</t>
   </si>
@@ -259,6 +259,72 @@
   </si>
   <si>
     <t>Charles Heller</t>
+  </si>
+  <si>
+    <t>one-way-anova</t>
+  </si>
+  <si>
+    <t>one-sample-t-test,dependent-samples-t-test,multiple-linear-regression</t>
+  </si>
+  <si>
+    <t>multiple-linear-regression</t>
+  </si>
+  <si>
+    <t>independent-samples-t-test,multiple-linear-regression,simple-linear-regression,dependent-samples-t-test</t>
+  </si>
+  <si>
+    <t>dependent-samples-t-test,one-sample-t-test</t>
+  </si>
+  <si>
+    <t>two-way-anova,one-way-anova</t>
+  </si>
+  <si>
+    <t>independent-samples-t-test</t>
+  </si>
+  <si>
+    <t>dependent-samples-t-test</t>
+  </si>
+  <si>
+    <t>simple-linear-regression,two-way-anova,independent-samples-t-test</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>0956797614545886.pdf (https://dl.airtable.com/sQiEblcHTzqA60UfEhKb_0956797614545886.pdf)</t>
+  </si>
+  <si>
+    <t>0956797615626691.pdf (https://dl.airtable.com/AKd7LiGUQVmsluL6mPKN_0956797615626691.pdf)</t>
+  </si>
+  <si>
+    <t>journal.pone.0182159.pdf (https://dl.airtable.com/9dKhg8EQnuaGoAtKob0d_journal.pone.0182159.pdf)</t>
+  </si>
+  <si>
+    <t>journal.pone.0182817.pdf (https://dl.airtable.com/Xer6TyfTS1yudPIFe5IL_journal.pone.0182817.pdf)</t>
+  </si>
+  <si>
+    <t>0956797614533801.pdf (https://dl.airtable.com/osAdTJQTUmMZjRkvevOk_0956797614533801.pdf)</t>
+  </si>
+  <si>
+    <t>journal.pone.0182239.pdf (https://dl.airtable.com/nAle73A2Rpy1JM4CMsQm_journal.pone.0182239.pdf)</t>
+  </si>
+  <si>
+    <t>journal.pone.0182907.pdf (https://dl.airtable.com/IZvp6MTPiGSoFZ8oeElA_journal.pone.0182907.pdf)</t>
+  </si>
+  <si>
+    <t>0956797615620784.pdf (https://dl.airtable.com/tfI9lhxORP2jJ1A0xwO2_0956797615620784.pdf)</t>
+  </si>
+  <si>
+    <t>journal.pone.0173493.pdf (https://dl.airtable.com/6N3azAFzROGVbLL6VvSB_journal.pone.0173493.pdf)</t>
+  </si>
+  <si>
+    <t>journal.pone.0177758.pdf (https://dl.airtable.com/9QV0nDO6SXqqzRKx18fg_journal.pone.0177758.pdf)</t>
+  </si>
+  <si>
+    <t>journal.pone.0152576.PDF (https://dl.airtable.com/P2I3CFfNTDmNV7nxo53h_journal.pone.0152576.PDF)</t>
+  </si>
+  <si>
+    <t>PDF(alternate link)</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,12 +1143,13 @@
     <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.5703125" customWidth="1"/>
     <col min="4" max="4" width="66" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="99.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="96.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1095,8 +1162,14 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1109,8 +1182,14 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1123,8 +1202,14 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1137,8 +1222,14 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1151,8 +1242,14 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1165,8 +1262,14 @@
       <c r="D6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1179,8 +1282,14 @@
       <c r="D7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1193,8 +1302,14 @@
       <c r="D8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1207,8 +1322,14 @@
       <c r="D9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1221,8 +1342,11 @@
       <c r="D10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1235,8 +1359,11 @@
       <c r="D11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1249,8 +1376,14 @@
       <c r="D12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1263,8 +1396,14 @@
       <c r="D13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1277,8 +1416,11 @@
       <c r="D14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1291,8 +1433,14 @@
       <c r="D15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1304,6 +1452,9 @@
       </c>
       <c r="D16" t="s">
         <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1315,8 +1466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,7 +2033,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,35 +2056,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1960,51 +2111,51 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C28">
-    <sortCondition ref="B2:B28"/>
+  <sortState ref="A2:C10">
+    <sortCondition ref="C2:C10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>